<commit_message>
committing code for Bit coin functionality
</commit_message>
<xml_diff>
--- a/cart_report.xlsx
+++ b/cart_report.xlsx
@@ -6,18 +6,27 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Cart Report" r:id="rId3" sheetId="1"/>
+    <sheet name="Report" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Report Summary</t>
+    <t>Cart Report Summary</t>
+  </si>
+  <si>
+    <t>Field</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
   <si>
     <t>Number of products added to the cart</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -62,11 +71,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="35.11328125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="6.09375" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -77,8 +90,16 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>1.0</v>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>